<commit_message>
[EDELIVERY-1966] - Commited new version of test projects + changed test suite for Bamboo v4
</commit_message>
<xml_diff>
--- a/Domibus-MSH-soapui-tests/src/main/soapui/reports/Domibus_3_2_2_test_results.xlsx
+++ b/Domibus-MSH-soapui-tests/src/main/soapui/reports/Domibus_3_2_2_test_results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1662" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1667" uniqueCount="446">
   <si>
     <t>NEED RUNNING - 3rd/green AC enabled</t>
   </si>
@@ -1358,6 +1358,15 @@
   </si>
   <si>
     <t>13.737s</t>
+  </si>
+  <si>
+    <t>0.139s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03-03-2017 17:07:52: Test case FAILED on step 1: Submit Message|| Returned error message[s]: 
+ |[Not SOAP Fault] Response is a SOAP Fault| 
+ |[XPath Match] XPathContains comparison failed for path [exists(//messageID)], expecting [true], actual was [false]| 
+ |[Script Assertion] Error:findReturnedMessageID: The message ID is not found in the response. Expression: (messageID != null). Values: messageID = null| </t>
   </si>
 </sst>
 </file>
@@ -2814,17 +2823,17 @@
         <v>0</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="H4" s="15">
-        <v>42795.467617152775</v>
+        <v>138</v>
+      </c>
+      <c r="H4" s="15" t="n">
+        <v>42797.71380347222</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>408</v>
+        <v>444</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1" t="s">
-        <v>384</v>
+        <v>445</v>
       </c>
       <c r="M4" s="7" t="s">
         <v>237</v>

</xml_diff>

<commit_message>
[EDELIVERY-1966] - Commited new version of test projects + changed test suite for Bamboo v5
</commit_message>
<xml_diff>
--- a/Domibus-MSH-soapui-tests/src/main/soapui/reports/Domibus_3_2_2_test_results.xlsx
+++ b/Domibus-MSH-soapui-tests/src/main/soapui/reports/Domibus_3_2_2_test_results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1667" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1682" uniqueCount="451">
   <si>
     <t>NEED RUNNING - 3rd/green AC enabled</t>
   </si>
@@ -1367,6 +1367,23 @@
  |[Not SOAP Fault] Response is a SOAP Fault| 
  |[XPath Match] XPathContains comparison failed for path [exists(//messageID)], expecting [true], actual was [false]| 
  |[Script Assertion] Error:findReturnedMessageID: The message ID is not found in the response. Expression: (messageID != null). Values: messageID = null| </t>
+  </si>
+  <si>
+    <t>1.083s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06-03-2017 11:12:43: Test case FAILED on step 1: Submit Message|| Returned error message[s]: 
+ |org.apache.http.conn.HttpHostConnectException: Connection to http://wltdgt02.cc.cec.eu.int:1063 refused| </t>
+  </si>
+  <si>
+    <t>1.021s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06-03-2017 11:29:09: Test case FAILED on step 1: Submit Message|| Returned error message[s]: 
+ |org.apache.http.conn.HttpHostConnectException: Connection to http://wltdgt02.cc.cec.eu.int:1063 refused| </t>
+  </si>
+  <si>
+    <t>2.347s</t>
   </si>
 </sst>
 </file>
@@ -2786,11 +2803,11 @@
       <c r="G3" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="H3" s="15">
-        <v>42795.467587094907</v>
+      <c r="H3" s="15" t="n">
+        <v>42800.659691967594</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>407</v>
+        <v>450</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="13" t="s">

</xml_diff>

<commit_message>
[EDELIVERY-1966] - Commited new version of test projects + changed test suite for Bamboo v5 - try with whole test suite
</commit_message>
<xml_diff>
--- a/Domibus-MSH-soapui-tests/src/main/soapui/reports/Domibus_3_2_2_test_results.xlsx
+++ b/Domibus-MSH-soapui-tests/src/main/soapui/reports/Domibus_3_2_2_test_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="20940" windowHeight="9855" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="20940" windowHeight="9855"/>
   </bookViews>
   <sheets>
     <sheet name="TESTS_WS" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1682" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1647" uniqueCount="440">
   <si>
     <t>NEED RUNNING - 3rd/green AC enabled</t>
   </si>
@@ -1246,12 +1246,6 @@
     <t>0.686s</t>
   </si>
   <si>
-    <t>2.261s</t>
-  </si>
-  <si>
-    <t>2.128s</t>
-  </si>
-  <si>
     <t>12.366s</t>
   </si>
   <si>
@@ -1327,63 +1321,28 @@
     <t>18.212s</t>
   </si>
   <si>
-    <t>4.953s</t>
-  </si>
-  <si>
     <t>2.214s</t>
   </si>
   <si>
     <t>2.12s</t>
   </si>
   <si>
-    <t>7.016s</t>
-  </si>
-  <si>
     <t>0.113s</t>
   </si>
   <si>
     <t>4.197s</t>
   </si>
   <si>
-    <t>0.25s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02-03-2017 09:52:42: Test case FAILED on step 1: Submit Message|| Returned error message[s]: 
- |[Not SOAP Fault] Response is a SOAP Fault| 
- |[XPath Match] XPathContains comparison failed for path [exists(//messageID)], expecting [true], actual was [false]| 
- |[Script Assertion] Error:findReturnedMessageID: The message ID is not found in the response. Expression: (messageID != null). Values: messageID = null| </t>
-  </si>
-  <si>
     <t>7.218s</t>
   </si>
   <si>
     <t>13.737s</t>
   </si>
   <si>
-    <t>0.139s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03-03-2017 17:07:52: Test case FAILED on step 1: Submit Message|| Returned error message[s]: 
- |[Not SOAP Fault] Response is a SOAP Fault| 
- |[XPath Match] XPathContains comparison failed for path [exists(//messageID)], expecting [true], actual was [false]| 
- |[Script Assertion] Error:findReturnedMessageID: The message ID is not found in the response. Expression: (messageID != null). Values: messageID = null| </t>
-  </si>
-  <si>
-    <t>1.083s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06-03-2017 11:12:43: Test case FAILED on step 1: Submit Message|| Returned error message[s]: 
- |org.apache.http.conn.HttpHostConnectException: Connection to http://wltdgt02.cc.cec.eu.int:1063 refused| </t>
-  </si>
-  <si>
-    <t>1.021s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06-03-2017 11:29:09: Test case FAILED on step 1: Submit Message|| Returned error message[s]: 
- |org.apache.http.conn.HttpHostConnectException: Connection to http://wltdgt02.cc.cec.eu.int:1063 refused| </t>
-  </si>
-  <si>
     <t>2.347s</t>
+  </si>
+  <si>
+    <t>3.504s</t>
   </si>
 </sst>
 </file>
@@ -2685,26 +2644,26 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O179"/>
   <sheetViews>
-    <sheetView topLeftCell="A132" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D171" sqref="D171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="76.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="97.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="64.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="33.42578125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="76.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="97.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="64.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="33.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="37.5" x14ac:dyDescent="0.3">
@@ -2803,11 +2762,11 @@
       <c r="G3" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="H3" s="15" t="n">
+      <c r="H3" s="15">
         <v>42800.659691967594</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="13" t="s">
@@ -2840,17 +2799,17 @@
         <v>0</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="H4" s="15" t="n">
-        <v>42797.71380347222</v>
+        <v>137</v>
+      </c>
+      <c r="H4" s="15">
+        <v>42800.720185057871</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1" t="s">
-        <v>445</v>
+        <v>384</v>
       </c>
       <c r="M4" s="7" t="s">
         <v>237</v>
@@ -2981,7 +2940,7 @@
         <v>42795.467644259261</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1" t="s">
@@ -3057,7 +3016,7 @@
         <v>42795.467791226853</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1" t="s">
@@ -3126,7 +3085,7 @@
         <v>42795.467820625003</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1" t="s">
@@ -3206,7 +3165,7 @@
         <v>42795.467947743055</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1" t="s">
@@ -3301,7 +3260,7 @@
         <v>42795.468027395837</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1" t="s">
@@ -3425,7 +3384,7 @@
         <v>42795.468124953702</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
@@ -3779,7 +3738,7 @@
         <v>42795.468320856482</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1" t="s">
@@ -4191,7 +4150,7 @@
         <v>42795.46847284722</v>
       </c>
       <c r="I47" s="12" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="J47" s="1"/>
       <c r="K47" s="1" t="s">
@@ -4224,7 +4183,7 @@
         <v>42795.468527337965</v>
       </c>
       <c r="I48" s="12" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="J48" s="1"/>
       <c r="K48" s="1" t="s">
@@ -4406,7 +4365,7 @@
         <v>42795.468628888892</v>
       </c>
       <c r="I54" s="12" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="J54" s="1"/>
       <c r="K54" s="1" t="s">
@@ -4621,7 +4580,7 @@
         <v>42795.468828310186</v>
       </c>
       <c r="I61" s="12" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="J61" s="1"/>
       <c r="K61" s="1" t="s">
@@ -4712,7 +4671,7 @@
         <v>42795.468858101849</v>
       </c>
       <c r="I64" s="12" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="J64" s="1"/>
       <c r="K64" s="1" t="s">
@@ -4774,7 +4733,7 @@
         <v>42795.468907546296</v>
       </c>
       <c r="I66" s="12" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="J66" s="1"/>
       <c r="K66" s="1" t="s">
@@ -4807,7 +4766,7 @@
         <v>42795.468957175923</v>
       </c>
       <c r="I67" s="12" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="J67" s="1"/>
       <c r="K67" s="1" t="s">
@@ -4902,7 +4861,7 @@
         <v>42795.469054687499</v>
       </c>
       <c r="I70" s="12" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="J70" s="1"/>
       <c r="K70" s="1" t="s">
@@ -4964,7 +4923,7 @@
         <v>42795.469104629628</v>
       </c>
       <c r="I72" s="12" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="J72" s="1"/>
       <c r="K72" s="1" t="s">
@@ -4997,7 +4956,7 @@
         <v>42795.469153692131</v>
       </c>
       <c r="I73" s="12" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="J73" s="1"/>
       <c r="K73" s="1" t="s">
@@ -5030,7 +4989,7 @@
         <v>42795.469202349537</v>
       </c>
       <c r="I74" s="12" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J74" s="1"/>
       <c r="K74" s="1" t="s">
@@ -5092,7 +5051,7 @@
         <v>42795.469251168979</v>
       </c>
       <c r="I76" s="12" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="J76" s="1"/>
       <c r="K76" s="1" t="s">
@@ -5125,7 +5084,7 @@
         <v>42795.469300081022</v>
       </c>
       <c r="I77" s="12" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="J77" s="1"/>
       <c r="K77" s="1" t="s">
@@ -5158,7 +5117,7 @@
         <v>42795.469348888888</v>
       </c>
       <c r="I78" s="12" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="J78" s="1"/>
       <c r="K78" s="1" t="s">
@@ -5191,7 +5150,7 @@
         <v>42795.469399953705</v>
       </c>
       <c r="I79" s="12" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J79" s="1"/>
       <c r="K79" s="1" t="s">
@@ -5499,7 +5458,7 @@
         <v>42795.46964422454</v>
       </c>
       <c r="I89" s="12" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="J89" s="1"/>
       <c r="K89" s="1" t="s">
@@ -5561,7 +5520,7 @@
         <v>42795.469692928244</v>
       </c>
       <c r="I91" s="12" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="J91" s="1"/>
       <c r="K91" s="1" t="s">
@@ -5594,7 +5553,7 @@
         <v>42795.469759409723</v>
       </c>
       <c r="I92" s="12" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="J92" s="1"/>
       <c r="K92" s="1" t="s">
@@ -5627,7 +5586,7 @@
         <v>42795.469816620367</v>
       </c>
       <c r="I93" s="12" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="J93" s="1"/>
       <c r="K93" s="1" t="s">
@@ -5689,7 +5648,7 @@
         <v>42795.469818078702</v>
       </c>
       <c r="I95" s="12" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="J95" s="1"/>
       <c r="K95" s="1" t="s">
@@ -5722,7 +5681,7 @@
         <v>42795.469857812503</v>
       </c>
       <c r="I96" s="12" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="J96" s="1"/>
       <c r="K96" s="1" t="s">
@@ -5755,7 +5714,7 @@
         <v>42795.469918263887</v>
       </c>
       <c r="I97" s="12" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="J97" s="1"/>
       <c r="K97" s="1" t="s">
@@ -5877,7 +5836,7 @@
         <v>42795.469974733795</v>
       </c>
       <c r="I101" s="12" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="J101" s="1"/>
       <c r="K101" s="1" t="s">
@@ -5960,11 +5919,11 @@
       <c r="G104" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="H104" s="15" t="n">
-        <v>42796.41161730324</v>
+      <c r="H104" s="15">
+        <v>42796.411617303238</v>
       </c>
       <c r="I104" s="12" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="J104" s="1"/>
       <c r="K104" s="1" t="s">
@@ -6057,7 +6016,7 @@
         <v>42795.470304444447</v>
       </c>
       <c r="I107" s="12" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="J107" s="1"/>
       <c r="K107" s="1" t="s">
@@ -6090,7 +6049,7 @@
         <v>42795.470333715275</v>
       </c>
       <c r="I108" s="12" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="J108" s="1"/>
       <c r="K108" s="1" t="s">
@@ -6148,11 +6107,11 @@
       <c r="G110" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="H110" s="15" t="n">
+      <c r="H110" s="15">
         <v>42796.41281199074</v>
       </c>
       <c r="I110" s="12" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="J110" s="1"/>
       <c r="K110" s="1" t="s">
@@ -6243,7 +6202,7 @@
         <v>42795.47044730324</v>
       </c>
       <c r="I113" s="12" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="J113" s="1"/>
       <c r="K113" s="1" t="s">
@@ -6392,7 +6351,7 @@
         <v>42795.470449780092</v>
       </c>
       <c r="I118" s="12" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="J118" s="1"/>
       <c r="K118" s="1" t="s">
@@ -8199,26 +8158,26 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:O129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="76.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="97.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="64.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="33.42578125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="76.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="97.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="64.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="33.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="37.5" x14ac:dyDescent="0.3">

</xml_diff>